<commit_message>
Actualización CN 06 06
Actualización CN 06 06
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion06/Escaleta_CN_06_06_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion06/Escaleta_CN_06_06_CO.xlsx
@@ -16,9 +16,9 @@
     <sheet name="DATOS" sheetId="1" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$2:$U$42</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1010,16 +1010,34 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1059,24 +1077,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1385,9 +1385,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1415,94 +1415,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="16" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="J1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="K1" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="L1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="M1" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="41"/>
-      <c r="O1" s="29" t="s">
+      <c r="N1" s="47"/>
+      <c r="O1" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="P1" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="44" t="s">
+      <c r="Q1" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="48" t="s">
+      <c r="R1" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="44" t="s">
+      <c r="S1" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="46" t="s">
+      <c r="T1" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="44" t="s">
+      <c r="U1" s="29" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="16" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="36"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="42"/>
       <c r="M2" s="17" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="45"/>
-      <c r="T2" s="47"/>
-      <c r="U2" s="45"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="30"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -4582,16 +4582,8 @@
     <row r="283" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="284" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:U42">
-    <filterColumn colId="12" showButton="0"/>
-  </autoFilter>
+  <autoFilter ref="A2:U42"/>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4606,6 +4598,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>